<commit_message>
Added Pro lite test data sheet and updated other test data related to pro lite panels
</commit_message>
<xml_diff>
--- a/Test Data/Gallery_Ethernet_AttachedFunctionality_ProPanels.xlsx
+++ b/Test Data/Gallery_Ethernet_AttachedFunctionality_ProPanels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEFE508-4BAF-4810-8EEC-F60552DFB241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872B6343-57B6-4674-A5A2-F7732A98739A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
@@ -117,10 +117,10 @@
     <t>NGC-3476/T2352</t>
   </si>
   <si>
-    <t>NGC-3479/T2407</t>
-  </si>
-  <si>
     <t>Portugal Market</t>
+  </si>
+  <si>
+    <t>NGC-3479/T2407/T2508</t>
   </si>
 </sst>
 </file>
@@ -1033,13 +1033,13 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
@@ -1057,7 +1057,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -1079,7 +1079,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">

</xml_diff>